<commit_message>
Really the final one
</commit_message>
<xml_diff>
--- a/Sprint Backlog - Tasks-1 (1) (1).xlsx
+++ b/Sprint Backlog - Tasks-1 (1) (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncgre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2456B496-FD0D-4F3F-9BE6-0C06509B2635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B41E39-687E-47D5-A139-7E23442A716B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>Samuel Glover</t>
   </si>
   <si>
-    <t>Ramiro Alvarez-Cruz</t>
-  </si>
-  <si>
     <t>User Story #1: Guest Checkout</t>
   </si>
   <si>
@@ -398,10 +395,13 @@
     <t>Document all public endpoints</t>
   </si>
   <si>
-    <t>Review and update documentation after final implementation changes</t>
-  </si>
-  <si>
     <t>Create basic user/admin usage walkthrough</t>
+  </si>
+  <si>
+    <t>Nicholas Greco</t>
+  </si>
+  <si>
+    <t>Document sprint reviews and backlogs</t>
   </si>
 </sst>
 </file>
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -915,7 +915,7 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
@@ -955,11 +955,11 @@
     </row>
     <row r="5" spans="1:12" ht="13.2">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="10">
         <v>7</v>
@@ -991,11 +991,11 @@
     </row>
     <row r="6" spans="1:12" ht="13.2">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="10">
         <v>8</v>
@@ -1027,11 +1027,11 @@
     </row>
     <row r="7" spans="1:12" ht="13.2">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="10">
         <v>3</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4">
         <v>13</v>
@@ -1104,11 +1104,11 @@
     </row>
     <row r="9" spans="1:12" ht="13.2">
       <c r="A9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="10">
         <v>3</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="10" spans="1:12" ht="13.2">
       <c r="A10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9" t="s">
@@ -1176,11 +1176,11 @@
     </row>
     <row r="11" spans="1:12" ht="13.2">
       <c r="A11" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="10">
         <v>5</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4">
         <v>5</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="13" spans="1:12" ht="13.2">
       <c r="A13" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="s">
@@ -1289,11 +1289,11 @@
     </row>
     <row r="14" spans="1:12" ht="13.2">
       <c r="A14" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D14" s="10">
         <v>8</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="15" spans="1:12" ht="13.2">
       <c r="A15" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9" t="s">
@@ -1361,7 +1361,7 @@
     </row>
     <row r="16" spans="1:12" ht="13.2">
       <c r="A16" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9" t="s">
@@ -1397,7 +1397,7 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4">
         <v>8</v>
@@ -1438,11 +1438,11 @@
     </row>
     <row r="18" spans="1:12" ht="13.2">
       <c r="A18" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D18" s="10">
         <v>9</v>
@@ -1474,11 +1474,11 @@
     </row>
     <row r="19" spans="1:12" ht="13.2">
       <c r="A19" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="10">
         <v>6</v>
@@ -1510,11 +1510,11 @@
     </row>
     <row r="20" spans="1:12" ht="13.2">
       <c r="A20" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D20" s="10">
         <v>6</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="21" spans="1:12" ht="13.2">
       <c r="A21" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9" t="s">
@@ -1582,7 +1582,7 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="4">
         <v>3</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="23" spans="1:12" ht="13.2">
       <c r="A23" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="9" t="s">
@@ -1659,7 +1659,7 @@
     </row>
     <row r="24" spans="1:12" ht="13.2">
       <c r="A24" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="9" t="s">
@@ -1695,7 +1695,7 @@
     </row>
     <row r="25" spans="1:12" ht="13.2">
       <c r="A25" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="9" t="s">
@@ -1731,7 +1731,7 @@
     </row>
     <row r="26" spans="1:12" ht="13.2">
       <c r="A26" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="9" t="s">
@@ -1767,7 +1767,7 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="4">
         <v>3</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9" t="s">
@@ -1844,7 +1844,7 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="9" t="s">
@@ -1880,7 +1880,7 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="9" t="s">
@@ -1916,7 +1916,7 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="9" t="s">
@@ -1952,7 +1952,7 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="4">
         <v>3</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
@@ -2029,7 +2029,7 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="9" t="s">
@@ -2065,7 +2065,7 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="9" t="s">
@@ -2101,7 +2101,7 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9" t="s">
@@ -2137,7 +2137,7 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="4">
         <v>3</v>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="9" t="s">
@@ -2214,7 +2214,7 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="A39" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="9" t="s">
@@ -2250,11 +2250,11 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="9" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D40" s="10">
         <v>4</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="9" t="s">
@@ -2322,7 +2322,7 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42" s="4">
         <v>3</v>
@@ -2363,11 +2363,11 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="10">
         <v>6</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="9" t="s">
@@ -2435,7 +2435,7 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="9" t="s">
@@ -2471,11 +2471,11 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="9" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D46" s="10">
         <v>7</v>
@@ -2550,7 +2550,7 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K26 K27:K46" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:K46" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"To Do,Doing,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>